<commit_message>
Resistance is done. Start Music Scores. No Idea :-)
</commit_message>
<xml_diff>
--- a/codingame_scraper/expert.xlsx
+++ b/codingame_scraper/expert.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\OneDrive\Documents\Programmation\codingame_py\codingame_scraper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/codingame_py/codingame_scraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A8784AF-17AD-4138-9E94-59FB9266DCEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{3A8784AF-17AD-4138-9E94-59FB9266DCEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FC0F6DA-B658-4963-8936-03B8A6C35A45}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="0" windowWidth="25596" windowHeight="18576" xr2:uid="{56912327-29C3-4E55-A958-F89779D2E66C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{56912327-29C3-4E55-A958-F89779D2E66C}"/>
   </bookViews>
   <sheets>
     <sheet name="expert_20250202" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>titre</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>DONE</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>En cours</t>
   </si>
 </sst>
 </file>
@@ -226,12 +232,17 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -267,9 +278,9 @@
     <sortCondition descending="1" ref="B1:B45"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{545CC2F1-062E-49B7-A267-94F5D93C73F8}" uniqueName="1" name="titre" queryTableFieldId="1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{545CC2F1-062E-49B7-A267-94F5D93C73F8}" uniqueName="1" name="titre" queryTableFieldId="1" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{0972A0DA-354E-4D8C-A561-9CF599AC5C69}" uniqueName="2" name="nombre de participants" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{F1EF7B33-DB47-4AEB-A192-C53A2F28ED9D}" uniqueName="3" name="DONE" queryTableFieldId="3"/>
+    <tableColumn id="3" xr3:uid="{F1EF7B33-DB47-4AEB-A192-C53A2F28ED9D}" uniqueName="3" name="DONE" queryTableFieldId="3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -595,13 +606,14 @@
   <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -611,28 +623,34 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>4115</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
         <v>2121</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
@@ -640,7 +658,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>24</v>
       </c>
       <c r="B5">
@@ -648,7 +666,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -656,7 +674,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>42</v>
       </c>
       <c r="B7">
@@ -664,7 +682,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8">
@@ -672,7 +690,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>28</v>
       </c>
       <c r="B9">
@@ -680,7 +698,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
       <c r="B10">
@@ -688,7 +706,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>25</v>
       </c>
       <c r="B11">
@@ -696,7 +714,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>44</v>
       </c>
       <c r="B12">
@@ -704,7 +722,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>34</v>
       </c>
       <c r="B13">
@@ -712,7 +730,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>30</v>
       </c>
       <c r="B14">
@@ -720,7 +738,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>40</v>
       </c>
       <c r="B15">
@@ -728,7 +746,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>22</v>
       </c>
       <c r="B16">
@@ -736,7 +754,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>35</v>
       </c>
       <c r="B17">
@@ -744,7 +762,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18">
@@ -752,7 +770,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>37</v>
       </c>
       <c r="B19">
@@ -760,7 +778,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>12</v>
       </c>
       <c r="B20">
@@ -768,7 +786,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>14</v>
       </c>
       <c r="B21">
@@ -776,7 +794,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22">
@@ -784,7 +802,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23">
@@ -792,7 +810,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>33</v>
       </c>
       <c r="B24">
@@ -800,7 +818,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
       <c r="B25">
@@ -808,7 +826,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>45</v>
       </c>
       <c r="B26">
@@ -816,7 +834,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>13</v>
       </c>
       <c r="B27">
@@ -824,7 +842,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>17</v>
       </c>
       <c r="B28">
@@ -832,7 +850,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>38</v>
       </c>
       <c r="B29">
@@ -840,7 +858,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>32</v>
       </c>
       <c r="B30">
@@ -848,7 +866,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>26</v>
       </c>
       <c r="B31">
@@ -856,7 +874,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>39</v>
       </c>
       <c r="B32">
@@ -864,7 +882,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>16</v>
       </c>
       <c r="B33">
@@ -872,7 +890,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>36</v>
       </c>
       <c r="B34">
@@ -880,7 +898,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>9</v>
       </c>
       <c r="B35">
@@ -888,7 +906,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>15</v>
       </c>
       <c r="B36">
@@ -896,7 +914,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>20</v>
       </c>
       <c r="B37">
@@ -904,7 +922,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>41</v>
       </c>
       <c r="B38">
@@ -912,7 +930,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>10</v>
       </c>
       <c r="B39">
@@ -920,7 +938,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>29</v>
       </c>
       <c r="B40">
@@ -928,7 +946,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>43</v>
       </c>
       <c r="B41">
@@ -936,7 +954,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>11</v>
       </c>
       <c r="B42">
@@ -944,7 +962,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>31</v>
       </c>
       <c r="B43">
@@ -952,7 +970,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>8</v>
       </c>
       <c r="B44">
@@ -960,7 +978,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+      <c r="A45" t="s">
         <v>7</v>
       </c>
       <c r="B45">

</xml_diff>